<commit_message>
Aggiunto indice Gulpease nuove versioni dei documenti
</commit_message>
<xml_diff>
--- a/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/metriche/grafici/graficiProcessiSupporto.xlsx
+++ b/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/metriche/grafici/graficiProcessiSupporto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Università\Terzo anno\SWE\Progetto\Documentazione\DocumentazioneEsterna\PianoDiQualifica\res\ResocontoAttivitaDiVerifica\res\metriche\grafici\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A1DBBD-AE9A-4172-BF9A-E2C75E5F35BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C077686B-A9DD-42E2-A31B-924CC7A23472}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3440947A-BDC3-41E2-B8C4-C01620109B14}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="34">
   <si>
     <t>Indice Gulpease</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>PA</t>
+  </si>
+  <si>
+    <t>1.1.0</t>
+  </si>
+  <si>
+    <t>2.0.0</t>
   </si>
 </sst>
 </file>
@@ -680,7 +686,7 @@
                   <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>70</c:v>
@@ -692,10 +698,10 @@
                   <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1553,9 +1559,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Documentazione!$B$60:$B$63</c:f>
+              <c:f>Documentazione!$B$60:$B$65</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.1.0</c:v>
                 </c:pt>
@@ -1567,16 +1573,22 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Documentazione!$C$60:$C$63</c:f>
+              <c:f>Documentazione!$C$60:$C$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>59</c:v>
                 </c:pt>
@@ -1588,6 +1600,12 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1627,9 +1645,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Documentazione!$B$60:$B$63</c:f>
+              <c:f>Documentazione!$B$60:$B$65</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.1.0</c:v>
                 </c:pt>
@@ -1641,16 +1659,22 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Documentazione!$D$60:$D$63</c:f>
+              <c:f>Documentazione!$D$60:$D$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>40</c:v>
                 </c:pt>
@@ -1661,6 +1685,12 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
@@ -1701,9 +1731,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Documentazione!$B$60:$B$63</c:f>
+              <c:f>Documentazione!$B$60:$B$65</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.1.0</c:v>
                 </c:pt>
@@ -1715,16 +1745,22 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Documentazione!$E$60:$E$63</c:f>
+              <c:f>Documentazione!$E$60:$E$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>80</c:v>
                 </c:pt>
@@ -1735,6 +1771,12 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
@@ -2252,9 +2294,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Documentazione!$B$82:$B$85</c:f>
+              <c:f>Documentazione!$B$82:$B$87</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.1.0</c:v>
                 </c:pt>
@@ -2266,16 +2308,22 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Documentazione!$C$82:$C$85</c:f>
+              <c:f>Documentazione!$C$82:$C$87</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>60</c:v>
                 </c:pt>
@@ -2287,6 +2335,12 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2326,9 +2380,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Documentazione!$B$82:$B$85</c:f>
+              <c:f>Documentazione!$B$82:$B$87</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.1.0</c:v>
                 </c:pt>
@@ -2340,16 +2394,22 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Documentazione!$D$82:$D$85</c:f>
+              <c:f>Documentazione!$D$82:$D$87</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>40</c:v>
                 </c:pt>
@@ -2360,6 +2420,12 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
@@ -2400,9 +2466,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Documentazione!$B$82:$B$85</c:f>
+              <c:f>Documentazione!$B$82:$B$87</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.1.0</c:v>
                 </c:pt>
@@ -2414,16 +2480,22 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Documentazione!$E$82:$E$85</c:f>
+              <c:f>Documentazione!$E$82:$E$87</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>80</c:v>
                 </c:pt>
@@ -2434,6 +2506,12 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
@@ -2946,9 +3024,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Documentazione!$B$105:$B$107</c:f>
+              <c:f>Documentazione!$B$105:$B$109</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.1.0</c:v>
                 </c:pt>
@@ -2957,16 +3035,22 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Documentazione!$C$105:$C$107</c:f>
+              <c:f>Documentazione!$C$105:$C$109</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>70</c:v>
                 </c:pt>
@@ -2975,6 +3059,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3014,9 +3104,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Documentazione!$B$105:$B$107</c:f>
+              <c:f>Documentazione!$B$105:$B$109</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.1.0</c:v>
                 </c:pt>
@@ -3025,16 +3115,22 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Documentazione!$D$105:$D$107</c:f>
+              <c:f>Documentazione!$D$105:$D$109</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>40</c:v>
                 </c:pt>
@@ -3042,6 +3138,12 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
@@ -3082,9 +3184,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Documentazione!$B$105:$B$107</c:f>
+              <c:f>Documentazione!$B$105:$B$109</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.1.0</c:v>
                 </c:pt>
@@ -3093,16 +3195,22 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Documentazione!$E$105:$E$107</c:f>
+              <c:f>Documentazione!$E$105:$E$109</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>80</c:v>
                 </c:pt>
@@ -3110,6 +3218,12 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
@@ -3622,9 +3736,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Documentazione!$B$124:$B$126</c:f>
+              <c:f>Documentazione!$B$124:$B$128</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.1.0</c:v>
                 </c:pt>
@@ -3633,16 +3747,22 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Documentazione!$C$124:$C$126</c:f>
+              <c:f>Documentazione!$C$124:$C$128</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>64</c:v>
                 </c:pt>
@@ -3651,6 +3771,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>68</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3690,9 +3816,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Documentazione!$B$124:$B$126</c:f>
+              <c:f>Documentazione!$B$124:$B$128</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.1.0</c:v>
                 </c:pt>
@@ -3701,16 +3827,22 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Documentazione!$D$124:$D$126</c:f>
+              <c:f>Documentazione!$D$124:$D$128</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>40</c:v>
                 </c:pt>
@@ -3718,6 +3850,12 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
@@ -3758,9 +3896,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Documentazione!$B$124:$B$126</c:f>
+              <c:f>Documentazione!$B$124:$B$128</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.1.0</c:v>
                 </c:pt>
@@ -3769,16 +3907,22 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Documentazione!$E$124:$E$126</c:f>
+              <c:f>Documentazione!$E$124:$E$128</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>80</c:v>
                 </c:pt>
@@ -3786,6 +3930,12 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
@@ -4979,9 +5129,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Documentazione!$B$167:$B$169</c:f>
+              <c:f>Documentazione!$B$167:$B$171</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.1.0</c:v>
                 </c:pt>
@@ -4990,16 +5140,22 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Documentazione!$C$167:$C$169</c:f>
+              <c:f>Documentazione!$C$167:$C$171</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>60</c:v>
                 </c:pt>
@@ -5007,6 +5163,12 @@
                   <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>59</c:v>
                 </c:pt>
               </c:numCache>
@@ -5047,9 +5209,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Documentazione!$B$167:$B$169</c:f>
+              <c:f>Documentazione!$B$167:$B$171</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.1.0</c:v>
                 </c:pt>
@@ -5058,16 +5220,22 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Documentazione!$D$167:$D$169</c:f>
+              <c:f>Documentazione!$D$167:$D$171</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>40</c:v>
                 </c:pt>
@@ -5075,6 +5243,12 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
@@ -5115,9 +5289,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Documentazione!$B$167:$B$169</c:f>
+              <c:f>Documentazione!$B$167:$B$171</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.1.0</c:v>
                 </c:pt>
@@ -5126,16 +5300,22 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Documentazione!$E$167:$E$169</c:f>
+              <c:f>Documentazione!$E$167:$E$171</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>80</c:v>
                 </c:pt>
@@ -5143,6 +5323,12 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
@@ -10977,8 +11163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67AECFA2-8686-4F57-8313-C78888B00A1F}">
   <dimension ref="B2:P239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="L223" sqref="L223"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11042,7 +11228,7 @@
         <v>68</v>
       </c>
       <c r="D4" s="2">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -11141,7 +11327,7 @@
         <v>60</v>
       </c>
       <c r="D9" s="2">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -11160,7 +11346,7 @@
         <v>61</v>
       </c>
       <c r="D10" s="2">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -11378,12 +11564,37 @@
       <c r="F63" s="13"/>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B64" s="8"/>
+      <c r="B64" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C64" s="2">
+        <v>60</v>
+      </c>
+      <c r="D64" s="2">
+        <v>40</v>
+      </c>
+      <c r="E64" s="2">
+        <v>80</v>
+      </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B65" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C65" s="2">
+        <v>65</v>
+      </c>
+      <c r="D65" s="2">
+        <v>40</v>
+      </c>
+      <c r="E65" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D71" s="5"/>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B80" s="1" t="s">
         <v>15</v>
       </c>
@@ -11465,6 +11676,34 @@
       </c>
       <c r="F85" s="13"/>
     </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B86" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C86" s="2">
+        <v>72</v>
+      </c>
+      <c r="D86" s="2">
+        <v>40</v>
+      </c>
+      <c r="E86" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B87" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C87" s="2">
+        <v>71</v>
+      </c>
+      <c r="D87" s="2">
+        <v>40</v>
+      </c>
+      <c r="E87" s="2">
+        <v>80</v>
+      </c>
+    </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B103" s="1" t="s">
         <v>19</v>
@@ -11532,6 +11771,34 @@
       </c>
       <c r="F107" s="13"/>
     </row>
+    <row r="108" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B108" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C108" s="2">
+        <v>70</v>
+      </c>
+      <c r="D108" s="2">
+        <v>40</v>
+      </c>
+      <c r="E108" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="109" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B109" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C109" s="2">
+        <v>70</v>
+      </c>
+      <c r="D109" s="2">
+        <v>40</v>
+      </c>
+      <c r="E109" s="2">
+        <v>80</v>
+      </c>
+    </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B122" s="1" t="s">
         <v>20</v>
@@ -11599,6 +11866,34 @@
       </c>
       <c r="F126" s="13"/>
     </row>
+    <row r="127" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B127" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C127" s="2">
+        <v>65</v>
+      </c>
+      <c r="D127" s="2">
+        <v>40</v>
+      </c>
+      <c r="E127" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="128" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B128" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C128" s="2">
+        <v>68</v>
+      </c>
+      <c r="D128" s="2">
+        <v>40</v>
+      </c>
+      <c r="E128" s="2">
+        <v>80</v>
+      </c>
+    </row>
     <row r="143" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B143" s="1" t="s">
         <v>21</v>
@@ -11732,6 +12027,34 @@
         <v>80</v>
       </c>
       <c r="F169" s="13"/>
+    </row>
+    <row r="170" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B170" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C170" s="2">
+        <v>60</v>
+      </c>
+      <c r="D170" s="2">
+        <v>40</v>
+      </c>
+      <c r="E170" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="171" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B171" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C171" s="2">
+        <v>59</v>
+      </c>
+      <c r="D171" s="2">
+        <v>40</v>
+      </c>
+      <c r="E171" s="2">
+        <v>80</v>
+      </c>
     </row>
     <row r="198" spans="2:8" ht="21" x14ac:dyDescent="0.4">
       <c r="E198" s="21" t="s">

</xml_diff>